<commit_message>
amos a por la blocal
</commit_message>
<xml_diff>
--- a/Tablas_MH2024.xlsx
+++ b/Tablas_MH2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrah\Documents\Universidad\Metaheurísticas\Practica1_Metaheuristicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEDAE15-7F76-45A4-B87D-E5EFEE82A2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC403B6E-7E5E-4DA1-A2F3-5549656305D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -112,6 +112,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -902,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -928,9 +931,6 @@
     <xf numFmtId="2" fontId="6" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -944,9 +944,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,86 +995,105 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="13" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,52 +1309,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M989"/>
+  <dimension ref="A1:O989"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10:N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" customWidth="1"/>
-    <col min="12" max="28" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="28" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="B1" s="44" t="s">
+    <row r="1" spans="1:15" ht="24" thickBot="1">
+      <c r="B1" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="44" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="44" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="44" t="s">
+      <c r="I1" s="54"/>
+      <c r="J1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="45"/>
+      <c r="K1" s="54"/>
     </row>
-    <row r="2" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:15" ht="13.5" customHeight="1">
+      <c r="A2" s="43" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1372,67 +1390,67 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="46" t="s">
+    <row r="3" spans="1:15" ht="15" customHeight="1">
+      <c r="A3" s="44"/>
+      <c r="B3" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="51">
         <v>2579</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="51">
         <v>6110</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="48">
+      <c r="G3" s="51">
         <v>58537</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="48">
+      <c r="I3" s="51">
         <v>645238</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="48">
+      <c r="K3" s="51">
         <v>224094</v>
       </c>
     </row>
-    <row r="4" spans="1:12" thickBot="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="49"/>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A4" s="44"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="52"/>
     </row>
-    <row r="5" spans="1:12" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="54"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="51"/>
+    <row r="5" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A5" s="44"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="37"/>
     </row>
-    <row r="6" spans="1:12" ht="16.8" thickBot="1">
-      <c r="A6" s="55"/>
+    <row r="6" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A6" s="45"/>
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1454,464 +1472,466 @@
       <c r="H6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="30" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N6" s="69"/>
+      <c r="O6" s="35"/>
     </row>
-    <row r="7" spans="1:12" ht="16.8" thickTop="1" thickBot="1">
+    <row r="7" spans="1:15" ht="17.25" thickTop="1" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="8">
         <v>28701.984642689298</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="57">
         <v>2.0978799999999999E-2</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>44737.941182747199</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="60">
         <v>6.2390000000000004E-4</v>
       </c>
       <c r="F7" s="8">
         <v>51351912.818514101</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="57">
         <v>1.0323761</v>
       </c>
-      <c r="H7" s="65">
+      <c r="H7" s="34">
         <v>674401.19093200203</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="61">
         <v>3.0299999999999999E-4</v>
       </c>
-      <c r="J7" s="36">
+      <c r="J7" s="31">
         <v>5590376.8554559303</v>
       </c>
-      <c r="K7" s="37">
+      <c r="K7" s="65">
         <v>2.1959000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16.2" thickBot="1">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="8">
         <v>29740.920425909098</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="57">
         <v>2.9202E-3</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>43103.945824336202</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="60">
         <v>6.2390000000000004E-4</v>
       </c>
       <c r="F8" s="8">
         <v>51354966.663442403</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="57">
         <v>1.0255780000000001</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>631935.55629429698</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="62">
         <v>1.471E-4</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="32">
         <v>5484160.2724685799</v>
       </c>
-      <c r="K8" s="43">
+      <c r="K8" s="66">
         <v>2.1226000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.2" thickBot="1">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="8">
         <v>28560.158514773801</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="57">
         <v>1.4302E-3</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>40208.896261267102</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="60">
         <v>5.4719999999999997E-4</v>
       </c>
       <c r="F9" s="8">
         <v>51164531.299697898</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="57">
         <v>0.97875190000000001</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>656080.79336170806</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="62">
         <v>1.6029999999999999E-4</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="32">
         <v>5697241.61440254</v>
       </c>
-      <c r="K9" s="43">
+      <c r="K9" s="66">
         <v>2.4497999999999998E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16.2" thickBot="1">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="8">
         <v>29914.635391732601</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="57">
         <v>8.9579999999999998E-4</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>42782.732407300398</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="60">
         <v>6.4720000000000001E-4</v>
       </c>
       <c r="F10" s="8">
         <v>51590479.330098704</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="57">
         <v>0.43566919999999998</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>696059.44136461301</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="63">
         <v>1.8870000000000001E-4</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="32">
         <v>5691895.07892296</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10" s="67">
         <v>2.2055999999999998E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.2" thickBot="1">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>29675.0637356078</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="58">
         <v>1.5074999999999999E-3</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="14">
         <v>43813.640235156701</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="59">
         <v>9.0350000000000001E-4</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>51395126.011817597</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="58">
         <v>0.43512410000000001</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="15">
         <v>652099.927325789</v>
       </c>
-      <c r="I11" s="35">
+      <c r="I11" s="64">
         <v>2.253E-4</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="33">
         <v>5690500.6991873197</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="68">
         <v>2.4239000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16.8" thickTop="1" thickBot="1">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:15" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="17">
         <f>AVERAGE((B7-C$3)/C$3,(B8-C$3)/C$3,(B9-C$3)/C$3,(B10-C$3)/C$3,(B11-C$3)/C$3)</f>
         <v>10.368186328864876</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="18">
         <f>AVERAGE(C7:C11)</f>
         <v>5.5464999999999993E-3</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="17">
         <f>AVERAGE((D7-E$3)/E$3,(D8-E$3)/E$3,(D9-E$3)/E$3,(D10-E$3)/E$3,(D11-E$3)/E$3)</f>
         <v>6.0260934831688244</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="18">
         <f t="shared" ref="E12" si="0">AVERAGE(E7:E11)</f>
         <v>6.6914000000000003E-4</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="17">
         <f t="shared" ref="F12" si="1">AVERAGE((F7-G$3)/G$3,(F8-G$3)/G$3,(F9-G$3)/G$3,(F10-G$3)/G$3,(F11-G$3)/G$3)</f>
         <v>876.58858883636242</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="18">
         <f t="shared" ref="G12" si="2">AVERAGE(G7:G11)</f>
         <v>0.78149985999999994</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="17">
         <f t="shared" ref="H12" si="3">AVERAGE((H7-I$3)/I$3,(H8-I$3)/I$3,(H9-I$3)/I$3,(H10-I$3)/I$3,(H11-I$3)/I$3)</f>
         <v>2.6156831829002351E-2</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="18">
         <f t="shared" ref="I12" si="4">AVERAGE(I7:I11)</f>
         <v>2.0488E-4</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="17">
         <f t="shared" ref="J12" si="5">AVERAGE((J7-K$3)/K$3,(J8-K$3)/K$3,(J9-K$3)/K$3,(J10-K$3)/K$3,(J11-K$3)/K$3)</f>
         <v>24.127111408995624</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="18">
         <f t="shared" ref="K12" si="6">AVERAGE(K7:K11)</f>
         <v>2.2795599999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16.2" thickBot="1">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="19">
         <f>STDEV((B7-C$3)/C$3,(B8-C$3)/C$3,(B9-C$3)/C$3,(B10-C$3)/C$3,(B11-C$3)/C$3)</f>
         <v>0.24646566045840734</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="19">
         <f>STDEV(C7:C11)</f>
         <v>8.6593849689224466E-3</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="19">
         <f t="shared" ref="D13" si="7">STDEV((D7-E$3)/E$3,(D8-E$3)/E$3,(D9-E$3)/E$3,(D10-E$3)/E$3,(D11-E$3)/E$3)</f>
         <v>0.27757962580882423</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="19">
         <f t="shared" ref="E13" si="8">STDEV(E7:E11)</f>
         <v>1.3635308210671295E-4</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="19">
         <f t="shared" ref="F13" si="9">STDEV((F7-G$3)/G$3,(F8-G$3)/G$3,(F9-G$3)/G$3,(F10-G$3)/G$3,(F11-G$3)/G$3)</f>
         <v>2.5908416432743091</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="19">
         <f t="shared" ref="G13" si="10">STDEV(G7:G11)</f>
         <v>0.31662138510300142</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="19">
         <f t="shared" ref="H13" si="11">STDEV((H7-I$3)/I$3,(H8-I$3)/I$3,(H9-I$3)/I$3,(H10-I$3)/I$3,(H11-I$3)/I$3)</f>
         <v>3.757054880836961E-2</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="19">
         <f t="shared" ref="I13" si="12">STDEV(I7:I11)</f>
         <v>6.2514414337814917E-5</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="19">
         <f t="shared" ref="J13" si="13">STDEV((J7-K$3)/K$3,(J8-K$3)/K$3,(J9-K$3)/K$3,(J10-K$3)/K$3,(J11-K$3)/K$3)</f>
         <v>0.41651615275903736</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="19">
         <f t="shared" ref="K13" si="14">STDEV(K7:K11)</f>
         <v>1.4741201782758411E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="25.8">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:15" ht="26.25">
+      <c r="A15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="66"/>
+      <c r="L15" s="35"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" thickBot="1"/>
     <row r="18" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A18" s="56"/>
-      <c r="B18" s="58" t="s">
+      <c r="A18" s="46"/>
+      <c r="B18" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="52" t="s">
+      <c r="C18" s="41"/>
+      <c r="D18" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="60" t="s">
+      <c r="E18" s="37"/>
+      <c r="F18" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="59"/>
-      <c r="H18" s="52" t="s">
+      <c r="G18" s="41"/>
+      <c r="H18" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="51"/>
-      <c r="J18" s="52" t="s">
+      <c r="I18" s="37"/>
+      <c r="J18" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="51"/>
-      <c r="L18" s="62" t="s">
+      <c r="K18" s="37"/>
+      <c r="L18" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="63"/>
+      <c r="M18" s="39"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A19" s="57"/>
-      <c r="B19" s="30" t="s">
+      <c r="A19" s="47"/>
+      <c r="B19" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="28" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="28" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="30" t="s">
+      <c r="J19" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="24" t="s">
+      <c r="M19" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="19">
         <f>B12</f>
         <v>10.368186328864876</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="70">
         <f t="shared" ref="C20:K20" si="15">C12</f>
         <v>5.5464999999999993E-3</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="19">
         <f t="shared" si="15"/>
         <v>6.0260934831688244</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="70">
         <f t="shared" si="15"/>
         <v>6.6914000000000003E-4</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="19">
         <f t="shared" si="15"/>
         <v>876.58858883636242</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="70">
         <f t="shared" si="15"/>
         <v>0.78149985999999994</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="19">
         <f t="shared" si="15"/>
         <v>2.6156831829002351E-2</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="70">
         <f t="shared" si="15"/>
         <v>2.0488E-4</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="19">
         <f t="shared" si="15"/>
         <v>24.127111408995624</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="70">
         <f t="shared" si="15"/>
         <v>2.2795599999999999E-3</v>
       </c>
-      <c r="L20" s="26">
+      <c r="L20" s="24">
         <f>AVERAGE(B20,D20,F20,H20,J20)</f>
         <v>183.42722737784413</v>
       </c>
-      <c r="M20" s="26">
+      <c r="M20" s="71">
         <f>AVERAGE(C20,E20,G20,I20,K20)</f>
         <v>0.15803998799999996</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="27"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="22"/>
+      <c r="A25" s="20"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="22"/>
+      <c r="A26" s="20"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:13" ht="15.75" customHeight="1"/>
@@ -2878,18 +2898,11 @@
     <row r="989" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J18:K18"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -2901,11 +2914,18 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
A por la tabú
</commit_message>
<xml_diff>
--- a/Tablas_MH2024.xlsx
+++ b/Tablas_MH2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrah\Documents\Universidad\Metaheurísticas\Practica1_Metaheuristicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D19CBA0-41A2-4254-A127-B3E7F86F7899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF367680-B4C0-4832-BDA9-A740E0DA964A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="25">
   <si>
     <t>Tamaño</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>BLocal</t>
+  </si>
+  <si>
+    <t>Tabú</t>
   </si>
 </sst>
 </file>
@@ -245,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -901,11 +904,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1052,8 +1068,10 @@
     <xf numFmtId="164" fontId="6" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1062,13 +1080,26 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1077,25 +1108,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1315,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O989"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1338,29 +1366,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24" thickBot="1">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="52" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="52" t="s">
+      <c r="E1" s="67"/>
+      <c r="F1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="52" t="s">
+      <c r="G1" s="67"/>
+      <c r="H1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="53"/>
-      <c r="J1" s="52" t="s">
+      <c r="I1" s="67"/>
+      <c r="J1" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="53"/>
+      <c r="K1" s="67"/>
     </row>
     <row r="2" spans="1:15" ht="13.5" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="68" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1395,7 +1423,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
-      <c r="A3" s="62"/>
+      <c r="A3" s="69"/>
       <c r="B3" s="54" t="s">
         <v>21</v>
       </c>
@@ -1428,7 +1456,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" thickBot="1">
-      <c r="A4" s="62"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="55"/>
       <c r="C4" s="57"/>
       <c r="D4" s="55"/>
@@ -1441,20 +1469,20 @@
       <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="59"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="61"/>
     </row>
     <row r="6" spans="1:15" ht="16.8" thickBot="1">
-      <c r="A6" s="63"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1760,29 +1788,29 @@
     <row r="16" spans="1:15" ht="13.8" customHeight="1"/>
     <row r="17" spans="1:11" ht="32.4" customHeight="1" thickBot="1">
       <c r="A17" s="36"/>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="52" t="s">
+      <c r="C17" s="67"/>
+      <c r="D17" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="52" t="s">
+      <c r="E17" s="67"/>
+      <c r="F17" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="53"/>
-      <c r="H17" s="52" t="s">
+      <c r="G17" s="67"/>
+      <c r="H17" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="53"/>
-      <c r="J17" s="52" t="s">
+      <c r="I17" s="67"/>
+      <c r="J17" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="53"/>
+      <c r="K17" s="67"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="68" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1817,7 +1845,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A19" s="62"/>
+      <c r="A19" s="69"/>
       <c r="B19" s="54" t="s">
         <v>21</v>
       </c>
@@ -1850,7 +1878,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="62"/>
+      <c r="A20" s="69"/>
       <c r="B20" s="55"/>
       <c r="C20" s="57"/>
       <c r="D20" s="55"/>
@@ -1863,20 +1891,20 @@
       <c r="K20" s="57"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A21" s="62"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="59"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="61"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A22" s="63"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="4" t="s">
         <v>1</v>
       </c>
@@ -1912,176 +1940,76 @@
       <c r="A23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="8">
-        <v>20218.355547961</v>
-      </c>
-      <c r="C23" s="37">
-        <v>0.42654530000000002</v>
-      </c>
-      <c r="D23" s="9">
-        <v>26942.656764548501</v>
-      </c>
-      <c r="E23" s="40">
-        <v>0.21167849999999999</v>
-      </c>
-      <c r="F23" s="8">
-        <v>32911671.0824674</v>
-      </c>
-      <c r="G23" s="37">
-        <v>3.6097714999999999</v>
-      </c>
-      <c r="H23" s="34">
-        <v>452541.165140889</v>
-      </c>
-      <c r="I23" s="41">
-        <v>0.16984399999999999</v>
-      </c>
-      <c r="J23" s="31">
-        <v>3526085.3152646399</v>
-      </c>
-      <c r="K23" s="45">
-        <v>0.61242859999999999</v>
-      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="45"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="8">
-        <v>19506.3524991993</v>
-      </c>
-      <c r="C24" s="37">
-        <v>0.3130754</v>
-      </c>
-      <c r="D24" s="9">
-        <v>25420.342733420399</v>
-      </c>
-      <c r="E24" s="40">
-        <v>0.17386399999999999</v>
-      </c>
-      <c r="F24" s="8">
-        <v>33114617.619410001</v>
-      </c>
-      <c r="G24" s="37">
-        <v>3.0334158000000002</v>
-      </c>
-      <c r="H24" s="10">
-        <v>432776.78652722598</v>
-      </c>
-      <c r="I24" s="42">
-        <v>0.17493529999999999</v>
-      </c>
-      <c r="J24" s="32">
-        <v>3477014.8693677699</v>
-      </c>
-      <c r="K24" s="46">
-        <v>0.55912490000000004</v>
-      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="46"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="8">
-        <v>19053.7790360422</v>
-      </c>
-      <c r="C25" s="37">
-        <v>0.2378622</v>
-      </c>
-      <c r="D25" s="9">
-        <v>26470.481299204399</v>
-      </c>
-      <c r="E25" s="40">
-        <v>0.15642819999999999</v>
-      </c>
-      <c r="F25" s="8">
-        <v>32648075.1653313</v>
-      </c>
-      <c r="G25" s="37">
-        <v>2.8487005999999999</v>
-      </c>
-      <c r="H25" s="10">
-        <v>459837.27367603499</v>
-      </c>
-      <c r="I25" s="42">
-        <v>0.1368365</v>
-      </c>
-      <c r="J25" s="32">
-        <v>3527870.8662961102</v>
-      </c>
-      <c r="K25" s="46">
-        <v>0.52843090000000004</v>
-      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="46"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="8">
-        <v>19834.0501876792</v>
-      </c>
-      <c r="C26" s="37">
-        <v>0.23555809999999999</v>
-      </c>
-      <c r="D26" s="9">
-        <v>25307.0759611787</v>
-      </c>
-      <c r="E26" s="40">
-        <v>0.12861149999999999</v>
-      </c>
-      <c r="F26" s="8">
-        <v>33226802.269450501</v>
-      </c>
-      <c r="G26" s="37">
-        <v>2.4199326999999999</v>
-      </c>
-      <c r="H26" s="10">
-        <v>434276.78868186497</v>
-      </c>
-      <c r="I26" s="43">
-        <v>0.13220470000000001</v>
-      </c>
-      <c r="J26" s="32">
-        <v>3594605.19533042</v>
-      </c>
-      <c r="K26" s="47">
-        <v>0.45996920000000002</v>
-      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="47"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="13">
-        <v>20029.219763308101</v>
-      </c>
-      <c r="C27" s="38">
-        <v>0.47776849999999998</v>
-      </c>
-      <c r="D27" s="14">
-        <v>24406.403356258699</v>
-      </c>
-      <c r="E27" s="39">
-        <v>0.13439019999999999</v>
-      </c>
-      <c r="F27" s="13">
-        <v>32849514.181116</v>
-      </c>
-      <c r="G27" s="38">
-        <v>2.9752458000000002</v>
-      </c>
-      <c r="H27" s="15">
-        <v>442760.07491293899</v>
-      </c>
-      <c r="I27" s="44">
-        <v>0.1395748</v>
-      </c>
-      <c r="J27" s="33">
-        <v>3697453.0339311301</v>
-      </c>
-      <c r="K27" s="48">
-        <v>0.43446069999999998</v>
-      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="48"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A28" s="16" t="s">
@@ -2089,43 +2017,43 @@
       </c>
       <c r="B28" s="17">
         <f>AVERAGE((B23-C$3)/C$3,(B24-C$3)/C$3,(B25-C$3)/C$3,(B26-C$3)/C$3,(B27-C$3)/C$3)</f>
-        <v>6.6496127983086311</v>
-      </c>
-      <c r="C28" s="18">
+        <v>-1</v>
+      </c>
+      <c r="C28" s="18" t="e">
         <f>AVERAGE(C23:C27)</f>
-        <v>0.33816190000000002</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D28" s="17">
         <f>AVERAGE((D23-E$3)/E$3,(D24-E$3)/E$3,(D25-E$3)/E$3,(D26-E$3)/E$3,(D27-E$3)/E$3)</f>
-        <v>3.2077564685633617</v>
-      </c>
-      <c r="E28" s="18">
+        <v>-1</v>
+      </c>
+      <c r="E28" s="18" t="e">
         <f t="shared" ref="E28" si="15">AVERAGE(E23:E27)</f>
-        <v>0.16099448</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F28" s="17">
         <f t="shared" ref="F28" si="16">AVERAGE((F23-G$3)/G$3,(F24-G$3)/G$3,(F25-G$3)/G$3,(F26-G$3)/G$3,(F27-G$3)/G$3)</f>
-        <v>50.066639075124286</v>
-      </c>
-      <c r="G28" s="18">
+        <v>-1</v>
+      </c>
+      <c r="G28" s="18" t="e">
         <f t="shared" ref="G28" si="17">AVERAGE(G23:G27)</f>
-        <v>2.9774132799999999</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H28" s="17">
         <f t="shared" ref="H28" si="18">AVERAGE((H23-I$3)/I$3,(H24-I$3)/I$3,(H25-I$3)/I$3,(H26-I$3)/I$3,(H27-I$3)/I$3)</f>
-        <v>6.5924358574541015</v>
-      </c>
-      <c r="I28" s="18">
+        <v>-1</v>
+      </c>
+      <c r="I28" s="18" t="e">
         <f t="shared" ref="I28" si="19">AVERAGE(I23:I27)</f>
-        <v>0.15067906000000003</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J28" s="17">
         <f t="shared" ref="J28" si="20">AVERAGE((J23-K$3)/K$3,(J24-K$3)/K$3,(J25-K$3)/K$3,(J26-K$3)/K$3,(J27-K$3)/K$3)</f>
-        <v>14.906743848733182</v>
-      </c>
-      <c r="K28" s="73">
+        <v>-1</v>
+      </c>
+      <c r="K28" s="53" t="e">
         <f t="shared" ref="K28" si="21">AVERAGE(K23:K27)</f>
-        <v>0.51888285999999995</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2134,281 +2062,582 @@
       </c>
       <c r="B29" s="19">
         <f>STDEV((B23-C$3)/C$3,(B24-C$3)/C$3,(B25-C$3)/C$3,(B26-C$3)/C$3,(B27-C$3)/C$3)</f>
-        <v>0.17833519852290813</v>
-      </c>
-      <c r="C29" s="19">
+        <v>0</v>
+      </c>
+      <c r="C29" s="19" t="e">
         <f>STDEV(C23:C27)</f>
-        <v>0.11013461108559383</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D29" s="19">
         <f t="shared" ref="D29" si="22">STDEV((D23-E$3)/E$3,(D24-E$3)/E$3,(D25-E$3)/E$3,(D26-E$3)/E$3,(D27-E$3)/E$3)</f>
-        <v>0.16455132912112741</v>
-      </c>
-      <c r="E29" s="19">
+        <v>0</v>
+      </c>
+      <c r="E29" s="19" t="e">
         <f t="shared" ref="E29" si="23">STDEV(E23:E27)</f>
-        <v>3.3584931328752017E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F29" s="19">
         <f t="shared" ref="F29" si="24">STDEV((F23-G$3)/G$3,(F24-G$3)/G$3,(F25-G$3)/G$3,(F26-G$3)/G$3,(F27-G$3)/G$3)</f>
-        <v>0.3520875345025955</v>
-      </c>
-      <c r="G29" s="19">
+        <v>0</v>
+      </c>
+      <c r="G29" s="19" t="e">
         <f t="shared" ref="G29" si="25">STDEV(G23:G27)</f>
-        <v>0.42730827562995644</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H29" s="19">
         <f t="shared" ref="H29" si="26">STDEV((H23-I$3)/I$3,(H24-I$3)/I$3,(H25-I$3)/I$3,(H26-I$3)/I$3,(H27-I$3)/I$3)</f>
-        <v>0.19937807920095393</v>
-      </c>
-      <c r="I29" s="19">
+        <v>0</v>
+      </c>
+      <c r="I29" s="19" t="e">
         <f t="shared" ref="I29" si="27">STDEV(I23:I27)</f>
-        <v>2.0074132229388888E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J29" s="19">
         <f t="shared" ref="J29" si="28">STDEV((J23-K$3)/K$3,(J24-K$3)/K$3,(J25-K$3)/K$3,(J26-K$3)/K$3,(J27-K$3)/K$3)</f>
-        <v>0.38031310269293711</v>
-      </c>
-      <c r="K29" s="19">
+        <v>0</v>
+      </c>
+      <c r="K29" s="19" t="e">
         <f t="shared" ref="K29" si="29">STDEV(K23:K27)</f>
-        <v>7.2559135808339503E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A33" s="64"/>
+    <row r="33" spans="1:11" ht="27.6" customHeight="1" thickBot="1">
+      <c r="A33" s="52"/>
       <c r="B33" s="66" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="67"/>
-      <c r="D33" s="60" t="s">
+      <c r="D33" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="59"/>
-      <c r="F33" s="68" t="s">
+      <c r="E33" s="67"/>
+      <c r="F33" s="66" t="s">
         <v>19</v>
       </c>
       <c r="G33" s="67"/>
-      <c r="H33" s="60" t="s">
+      <c r="H33" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="I33" s="59"/>
-      <c r="J33" s="60" t="s">
+      <c r="I33" s="67"/>
+      <c r="J33" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="K33" s="59"/>
-      <c r="L33" s="70" t="s">
+      <c r="K33" s="67"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A34" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>280</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>130</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>18512</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>144</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A35" s="69"/>
+      <c r="B35" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="56">
+        <v>2579</v>
+      </c>
+      <c r="D35" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="56">
+        <v>6110</v>
+      </c>
+      <c r="F35" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="56">
+        <v>645238</v>
+      </c>
+      <c r="H35" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="56">
+        <v>58537</v>
+      </c>
+      <c r="J35" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="56">
+        <v>224094</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A36" s="69"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="57"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A37" s="69"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="61"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A38" s="70"/>
+      <c r="B38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="J38" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="45"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A40" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="46"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="46"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A42" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="47"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="48"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A44" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="17">
+        <f>AVERAGE((B39-C$3)/C$3,(B40-C$3)/C$3,(B41-C$3)/C$3,(B42-C$3)/C$3,(B43-C$3)/C$3)</f>
+        <v>-1</v>
+      </c>
+      <c r="C44" s="18" t="e">
+        <f>AVERAGE(C39:C43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D44" s="17">
+        <f t="shared" ref="D44" si="30">AVERAGE((D39-E$3)/E$3,(D40-E$3)/E$3,(D41-E$3)/E$3,(D42-E$3)/E$3,(D43-E$3)/E$3)</f>
+        <v>-1</v>
+      </c>
+      <c r="E44" s="18" t="e">
+        <f t="shared" ref="E44" si="31">AVERAGE(E39:E43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F44" s="17">
+        <f t="shared" ref="F44" si="32">AVERAGE((F39-G$3)/G$3,(F40-G$3)/G$3,(F41-G$3)/G$3,(F42-G$3)/G$3,(F43-G$3)/G$3)</f>
+        <v>-1</v>
+      </c>
+      <c r="G44" s="18" t="e">
+        <f t="shared" ref="G44" si="33">AVERAGE(G39:G43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H44" s="17">
+        <f t="shared" ref="H44" si="34">AVERAGE((H39-I$3)/I$3,(H40-I$3)/I$3,(H41-I$3)/I$3,(H42-I$3)/I$3,(H43-I$3)/I$3)</f>
+        <v>-1</v>
+      </c>
+      <c r="I44" s="18" t="e">
+        <f t="shared" ref="I44" si="35">AVERAGE(I39:I43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J44" s="17">
+        <f t="shared" ref="J44" si="36">AVERAGE((J39-K$3)/K$3,(J40-K$3)/K$3,(J41-K$3)/K$3,(J42-K$3)/K$3,(J43-K$3)/K$3)</f>
+        <v>-1</v>
+      </c>
+      <c r="K44" s="18" t="e">
+        <f t="shared" ref="K44" si="37">AVERAGE(K39:K43)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A45" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="19">
+        <f>STDEV((B39-C$3)/C$3,(B40-C$3)/C$3,(B41-C$3)/C$3,(B42-C$3)/C$3,(B43-C$3)/C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="19" t="e">
+        <f>STDEV(C39:C43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D45" s="19">
+        <f t="shared" ref="D45:K45" si="38">STDEV((D39-E$3)/E$3,(D40-E$3)/E$3,(D41-E$3)/E$3,(D42-E$3)/E$3,(D43-E$3)/E$3)</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="19" t="e">
+        <f t="shared" ref="E45:K45" si="39">STDEV(E39:E43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F45" s="19">
+        <f t="shared" ref="F45:K45" si="40">STDEV((F39-G$3)/G$3,(F40-G$3)/G$3,(F41-G$3)/G$3,(F42-G$3)/G$3,(F43-G$3)/G$3)</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="19" t="e">
+        <f t="shared" ref="G45:K45" si="41">STDEV(G39:G43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H45" s="19">
+        <f t="shared" ref="H45:K45" si="42">STDEV((H39-I$3)/I$3,(H40-I$3)/I$3,(H41-I$3)/I$3,(H42-I$3)/I$3,(H43-I$3)/I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="19" t="e">
+        <f t="shared" ref="I45:K45" si="43">STDEV(I39:I43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J45" s="19">
+        <f t="shared" ref="J45:K45" si="44">STDEV((J39-K$3)/K$3,(J40-K$3)/K$3,(J41-K$3)/K$3,(J42-K$3)/K$3,(J43-K$3)/K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="K45" s="19" t="e">
+        <f t="shared" ref="K45" si="45">STDEV(K39:K43)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="49" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="50" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="51" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="52" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="53" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="55" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="56" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="58" spans="1:13" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="59" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A59" s="71"/>
+      <c r="B59" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="75"/>
+      <c r="D59" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="75"/>
+      <c r="F59" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="G59" s="75"/>
+      <c r="H59" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="I59" s="74"/>
+      <c r="J59" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="K59" s="77"/>
+      <c r="L59" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="M33" s="71"/>
-    </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A34" s="65"/>
-      <c r="B34" s="28" t="s">
+      <c r="M59" s="65"/>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A60" s="76"/>
+      <c r="B60" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D60" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E60" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="28" t="s">
+      <c r="F60" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G60" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H34" s="28" t="s">
+      <c r="H60" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I60" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J34" s="28" t="s">
+      <c r="J60" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="K60" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L34" s="21" t="s">
+      <c r="L60" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M34" s="22" t="s">
+      <c r="M60" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A35" s="23" t="s">
+    <row r="61" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A61" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="19">
+      <c r="B61" s="19">
         <f>B12</f>
         <v>10.368186328864876</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C61" s="50">
         <f>C12</f>
         <v>5.5464999999999993E-3</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D61" s="19">
         <f>D12</f>
         <v>6.0260934831688244</v>
       </c>
-      <c r="E35" s="50">
+      <c r="E61" s="50">
         <f>E12</f>
         <v>6.6914000000000003E-4</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F61" s="19">
         <f>F12</f>
         <v>78.61620863110069</v>
       </c>
-      <c r="G35" s="50">
+      <c r="G61" s="50">
         <f>G12</f>
         <v>0.78149985999999994</v>
       </c>
-      <c r="H35" s="19">
+      <c r="H61" s="19">
         <f>H12</f>
         <v>10.311057653376187</v>
       </c>
-      <c r="I35" s="50">
+      <c r="I61" s="50">
         <f>I12</f>
         <v>2.0488E-4</v>
       </c>
-      <c r="J35" s="19">
+      <c r="J61" s="19">
         <f>J12</f>
         <v>24.127111408995624</v>
       </c>
-      <c r="K35" s="50">
+      <c r="K61" s="50">
         <f>K12</f>
         <v>2.2795599999999999E-3</v>
       </c>
-      <c r="L35" s="24">
-        <f>AVERAGE(B35,D35,F35,H35,J35)</f>
+      <c r="L61" s="24">
+        <f>AVERAGE(B61,D61,F61,H61,J61)</f>
         <v>25.889731501101238</v>
       </c>
-      <c r="M35" s="51">
-        <f>AVERAGE(C35,E35,G35,I35,K35)</f>
+      <c r="M61" s="51">
+        <f>AVERAGE(C61,E61,G61,I61,K61)</f>
         <v>0.15803998799999996</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A36" s="23" t="s">
+    <row r="62" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A62" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B62" s="19">
         <f>B28</f>
-        <v>6.6496127983086311</v>
-      </c>
-      <c r="C36" s="19">
+        <v>-1</v>
+      </c>
+      <c r="C62" s="19" t="e">
         <f>C28</f>
-        <v>0.33816190000000002</v>
-      </c>
-      <c r="D36" s="19">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D62" s="19">
         <f>D28</f>
-        <v>3.2077564685633617</v>
-      </c>
-      <c r="E36" s="19">
+        <v>-1</v>
+      </c>
+      <c r="E62" s="19" t="e">
         <f>E28</f>
-        <v>0.16099448</v>
-      </c>
-      <c r="F36" s="19">
-        <f t="shared" ref="F36:K36" si="30">F28</f>
-        <v>50.066639075124286</v>
-      </c>
-      <c r="G36" s="19">
-        <f t="shared" si="30"/>
-        <v>2.9774132799999999</v>
-      </c>
-      <c r="H36" s="19">
-        <f t="shared" si="30"/>
-        <v>6.5924358574541015</v>
-      </c>
-      <c r="I36" s="19">
-        <f t="shared" si="30"/>
-        <v>0.15067906000000003</v>
-      </c>
-      <c r="J36" s="19">
-        <f t="shared" si="30"/>
-        <v>14.906743848733182</v>
-      </c>
-      <c r="K36" s="19">
-        <f t="shared" si="30"/>
-        <v>0.51888285999999995</v>
-      </c>
-      <c r="L36" s="24">
-        <f>AVERAGE(B36,D36,F36,H36,J36)</f>
-        <v>16.284637609636711</v>
-      </c>
-      <c r="M36" s="51">
-        <f>AVERAGE(C36,E36,G36,I36,K36)</f>
-        <v>0.82922631599999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A37" s="26" t="s">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F62" s="19">
+        <f>F28</f>
+        <v>-1</v>
+      </c>
+      <c r="G62" s="19" t="e">
+        <f>G28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H62" s="19">
+        <f>H28</f>
+        <v>-1</v>
+      </c>
+      <c r="I62" s="19" t="e">
+        <f>I28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J62" s="19">
+        <f>J28</f>
+        <v>-1</v>
+      </c>
+      <c r="K62" s="19" t="e">
+        <f>K28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L62" s="24">
+        <f>AVERAGE(B62,D62,F62,H62,J62)</f>
+        <v>-1</v>
+      </c>
+      <c r="M62" s="51" t="e">
+        <f>AVERAGE(C62,E62,G62,I62,K62)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A63" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="25"/>
-    </row>
-    <row r="38" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="26" t="s">
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="27"/>
+      <c r="J63" s="27"/>
+      <c r="K63" s="27"/>
+      <c r="L63" s="24"/>
+      <c r="M63" s="25"/>
+    </row>
+    <row r="64" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A64" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="25"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1" thickTop="1"/>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="24"/>
+      <c r="M64" s="25"/>
+    </row>
+    <row r="65" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
     <row r="68" ht="15.75" customHeight="1"/>
@@ -3334,18 +3563,54 @@
     <row r="988" ht="15.75" customHeight="1"/>
     <row r="989" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
+  <mergeCells count="70">
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
     <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="L59:M59"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="H5:I5"/>
@@ -3360,30 +3625,15 @@
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>